<commit_message>
Updated with yml based configuration
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_bdd_testcase_run_manager.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_bdd_testcase_run_manager.xlsx
@@ -177,11 +177,14 @@
   <si>
     <t>success=EXACT("available","[status]")</t>
   </si>
+  <si>
+    <t>code=MISSING_MOCK_DATA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" count="8" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
@@ -527,7 +530,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0" tabSelected="1">
-      <selection pane="topLeft" activeCell="L4" sqref="L4"/>
+      <selection pane="topLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -596,7 +599,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>

</xml_diff>